<commit_message>
Add Online Payment for blank payment method
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t>S. No.</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>angadsehgal@hotmail.com</t>
+  </si>
+  <si>
+    <t>Online Payment</t>
   </si>
   <si>
     <t xml:space="preserve">Ssss </t>
@@ -758,7 +761,7 @@
         <v>50</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="K4">
         <v>110.48</v>
@@ -772,13 +775,13 @@
         <v>36</v>
       </c>
       <c r="P4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q4">
         <v>110048</v>
       </c>
       <c r="R4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -786,7 +789,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>6046</v>
@@ -795,13 +798,13 @@
         <v>10648</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H5">
         <v>15</v>
@@ -818,13 +821,13 @@
       <c r="L5"/>
       <c r="M5"/>
       <c r="N5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O5" t="s">
         <v>36</v>
       </c>
       <c r="P5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q5">
         <v>111111</v>
@@ -880,7 +883,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>6049</v>
@@ -889,13 +892,13 @@
         <v>10628</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -912,13 +915,13 @@
       <c r="L6"/>
       <c r="M6"/>
       <c r="N6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q6">
         <v>111111</v>
@@ -935,7 +938,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C7">
         <v>6050</v>
@@ -944,13 +947,13 @@
         <v>5951</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -967,13 +970,13 @@
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q7">
         <v>110018</v>

</xml_diff>

<commit_message>
Add Phone number from Address table, time buffer
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="81">
   <si>
     <t>S. No.</t>
   </si>
@@ -71,21 +71,111 @@
     <t>Product Selection</t>
   </si>
   <si>
-    <t>2017-09-30 11:22:06</t>
+    <t>2017-09-26 18:05</t>
+  </si>
+  <si>
+    <t>Rohit Singh</t>
+  </si>
+  <si>
+    <t>8373934770</t>
+  </si>
+  <si>
+    <t>rohitrrr@gmail.com</t>
+  </si>
+  <si>
+    <t>Cash On Delivery</t>
+  </si>
+  <si>
+    <t>New Delhi, Delhi 110018</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/4, Najafgarh Rd, Block 1, Tilak Nagar </t>
+  </si>
+  <si>
+    <t>All in One Mixture (Weight: 100 Grams)</t>
+  </si>
+  <si>
+    <t>Chana Malai (Weight: 100 Grams)</t>
+  </si>
+  <si>
+    <t>Apricot (Weight: 50 Grams)</t>
+  </si>
+  <si>
+    <t>2017-09-27 18:48</t>
+  </si>
+  <si>
+    <t>rohit singh</t>
+  </si>
+  <si>
+    <t>rohit.dignitas100@gmail.com</t>
+  </si>
+  <si>
+    <t>Credit Card / Debit Card / Net Banking (Razorpay)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/4 Tilak Nagar </t>
+  </si>
+  <si>
+    <t>Brain Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apple Cinnamon Granola Bar (3 Bars) </t>
+  </si>
+  <si>
+    <t>2017-09-27 21:08</t>
+  </si>
+  <si>
+    <t>adada sadasd</t>
+  </si>
+  <si>
+    <t>08860327209</t>
+  </si>
+  <si>
+    <t>anela.kumar@gmail.com</t>
+  </si>
+  <si>
+    <t>sfsaf</t>
+  </si>
+  <si>
+    <t>Lakshadweep Islands</t>
+  </si>
+  <si>
+    <t>asfafs asfaf</t>
+  </si>
+  <si>
+    <t>2017-09-27 21:24</t>
+  </si>
+  <si>
+    <t>Fruity Fusion</t>
+  </si>
+  <si>
+    <t>Four Powerful Fruits</t>
+  </si>
+  <si>
+    <t>2017-09-27 22:20</t>
+  </si>
+  <si>
+    <t>2017-09-29 21:52</t>
+  </si>
+  <si>
+    <t>2017-09-29 22:04</t>
+  </si>
+  <si>
+    <t>2017-09-29 22:51</t>
+  </si>
+  <si>
+    <t>2017-09-30 23:52</t>
   </si>
   <si>
     <t>rrSS ss</t>
   </si>
   <si>
-    <t>8373934770</t>
-  </si>
-  <si>
     <t>rohit.dignitas121@gmail.com</t>
   </si>
   <si>
-    <t>Cash On Delivery</t>
-  </si>
-  <si>
     <t>new dfdd</t>
   </si>
   <si>
@@ -101,16 +191,10 @@
     <t>Assorted Instant Drink Pack</t>
   </si>
   <si>
-    <t>All in One Mixture (Weight: 100 Grams)</t>
-  </si>
-  <si>
-    <t>Apricot (Weight: 50 Grams)</t>
-  </si>
-  <si>
     <t>All in One Mixture -Test Product</t>
   </si>
   <si>
-    <t>2017-10-02 03:04:56</t>
+    <t>2017-10-02 15:34</t>
   </si>
   <si>
     <t>A Saaa</t>
@@ -125,16 +209,10 @@
     <t>delhi</t>
   </si>
   <si>
-    <t>Delhi</t>
-  </si>
-  <si>
     <t xml:space="preserve">gk-1  </t>
   </si>
   <si>
-    <t>Chana Malai (Weight: 100 Grams)</t>
-  </si>
-  <si>
-    <t>2017-10-02 15:53:22</t>
+    <t>2017-10-03 04:23</t>
   </si>
   <si>
     <t>Angad Sehgal</t>
@@ -152,7 +230,7 @@
     <t>Get Energized</t>
   </si>
   <si>
-    <t>2017-10-03 07:06:31</t>
+    <t>2017-10-03 19:36</t>
   </si>
   <si>
     <t>Rohit Dignitas</t>
@@ -167,28 +245,10 @@
     <t>Add ress 1  address 2</t>
   </si>
   <si>
-    <t>2017-10-03 09:07:28</t>
-  </si>
-  <si>
-    <t>adada sadasd</t>
-  </si>
-  <si>
-    <t>08860327209</t>
-  </si>
-  <si>
-    <t>anela.kumar@gmail.com</t>
-  </si>
-  <si>
-    <t>sfsaf</t>
-  </si>
-  <si>
-    <t>Lakshadweep Islands</t>
-  </si>
-  <si>
-    <t>asfafs asfaf</t>
-  </si>
-  <si>
-    <t>2017-10-03 09:08:54</t>
+    <t>2017-10-03 21:37</t>
+  </si>
+  <si>
+    <t>2017-10-03 21:38</t>
   </si>
   <si>
     <t xml:space="preserve">Rohit  Testing </t>
@@ -554,7 +614,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AF7"/>
+  <dimension ref="A1:AF15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="R1" sqref="R1"/>
@@ -626,10 +686,10 @@
         <v>18</v>
       </c>
       <c r="C2">
-        <v>6027</v>
+        <v>5953</v>
       </c>
       <c r="D2">
-        <v>10643</v>
+        <v>10617</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -641,16 +701,16 @@
         <v>21</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="J2" t="s">
         <v>22</v>
       </c>
       <c r="K2">
-        <v>220.12</v>
+        <v>208.1</v>
       </c>
       <c r="L2"/>
       <c r="M2"/>
@@ -664,7 +724,7 @@
         <v>25</v>
       </c>
       <c r="Q2">
-        <v>111111</v>
+        <v>110018</v>
       </c>
       <c r="R2" t="s">
         <v>26</v>
@@ -674,12 +734,6 @@
       </c>
       <c r="T2" t="s">
         <v>28</v>
-      </c>
-      <c r="U2" t="s">
-        <v>29</v>
-      </c>
-      <c r="V2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:32">
@@ -687,51 +741,60 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>5967</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
         <v>31</v>
       </c>
-      <c r="C3">
-        <v>6035</v>
-      </c>
-      <c r="D3">
-        <v>10645</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>200</v>
+      </c>
+      <c r="J3" t="s">
         <v>32</v>
       </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>100</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
       <c r="K3">
-        <v>90.32</v>
+        <v>35.4</v>
       </c>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3">
+        <v>110046</v>
+      </c>
+      <c r="R3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" t="s">
         <v>35</v>
       </c>
-      <c r="O3" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3">
-        <v>110048</v>
-      </c>
-      <c r="R3" t="s">
-        <v>38</v>
+      <c r="T3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:32">
@@ -739,49 +802,54 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>5969</v>
+      </c>
+      <c r="D4">
+        <v>10625</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
         <v>39</v>
       </c>
-      <c r="C4">
-        <v>6039</v>
-      </c>
-      <c r="D4">
-        <v>6551</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4"/>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
       <c r="H4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="K4">
-        <v>110.48</v>
+        <v>215.4</v>
       </c>
       <c r="L4"/>
       <c r="M4"/>
       <c r="N4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="O4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="P4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q4">
-        <v>110048</v>
+        <v>111111</v>
       </c>
       <c r="R4" t="s">
-        <v>44</v>
+        <v>35</v>
+      </c>
+      <c r="S4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -789,93 +857,54 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5">
-        <v>6046</v>
+        <v>5970</v>
       </c>
       <c r="D5">
-        <v>10648</v>
+        <v>10625</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H5">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>1300</v>
+        <v>100</v>
       </c>
       <c r="J5" t="s">
         <v>22</v>
       </c>
       <c r="K5">
-        <v>730.12</v>
+        <v>153.8</v>
       </c>
       <c r="L5"/>
       <c r="M5"/>
       <c r="N5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="P5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="Q5">
         <v>111111</v>
       </c>
       <c r="R5" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="S5" t="s">
-        <v>28</v>
-      </c>
-      <c r="T5" t="s">
-        <v>28</v>
-      </c>
-      <c r="U5" t="s">
-        <v>28</v>
-      </c>
-      <c r="V5" t="s">
-        <v>28</v>
-      </c>
-      <c r="W5" t="s">
-        <v>28</v>
-      </c>
-      <c r="X5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:32">
@@ -883,54 +912,54 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C6">
-        <v>6049</v>
+        <v>5971</v>
       </c>
       <c r="D6">
-        <v>10628</v>
+        <v>10625</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="J6" t="s">
         <v>22</v>
       </c>
       <c r="K6">
-        <v>162</v>
+        <v>215.4</v>
       </c>
       <c r="L6"/>
       <c r="M6"/>
       <c r="N6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="O6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="P6" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="Q6">
         <v>111111</v>
       </c>
       <c r="R6" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="S6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:32">
@@ -938,51 +967,545 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C7">
-        <v>6050</v>
+        <v>6003</v>
       </c>
       <c r="D7">
-        <v>5951</v>
+        <v>10628</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="J7" t="s">
         <v>22</v>
       </c>
       <c r="K7">
-        <v>100</v>
+        <v>280</v>
       </c>
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7">
+        <v>111111</v>
+      </c>
+      <c r="R7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="O7" t="s">
-        <v>48</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="C8">
+        <v>6007</v>
+      </c>
+      <c r="D8">
+        <v>10628</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
+      <c r="J8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8">
+        <v>106</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8">
+        <v>111111</v>
+      </c>
+      <c r="R8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <v>6010</v>
+      </c>
+      <c r="D9">
+        <v>10628</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>400</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9">
+        <v>224</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q9">
+        <v>111111</v>
+      </c>
+      <c r="R9" t="s">
+        <v>26</v>
+      </c>
+      <c r="S9" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" t="s">
+        <v>26</v>
+      </c>
+      <c r="U9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <v>6027</v>
+      </c>
+      <c r="D10">
+        <v>10643</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>225</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10">
+        <v>220.12</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10" t="s">
+        <v>53</v>
+      </c>
+      <c r="O10" t="s">
+        <v>54</v>
+      </c>
+      <c r="P10" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q10">
+        <v>111111</v>
+      </c>
+      <c r="R10" t="s">
+        <v>56</v>
+      </c>
+      <c r="S10" t="s">
+        <v>57</v>
+      </c>
+      <c r="T10" t="s">
+        <v>26</v>
+      </c>
+      <c r="U10" t="s">
+        <v>28</v>
+      </c>
+      <c r="V10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11">
+        <v>6035</v>
+      </c>
+      <c r="D11">
+        <v>10645</v>
+      </c>
+      <c r="E11" t="s">
         <v>60</v>
       </c>
-      <c r="Q7">
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11">
+        <v>90.32</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11" t="s">
+        <v>63</v>
+      </c>
+      <c r="O11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q11">
+        <v>110048</v>
+      </c>
+      <c r="R11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12">
+        <v>6039</v>
+      </c>
+      <c r="D12">
+        <v>6551</v>
+      </c>
+      <c r="E12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12">
+        <v>12345</v>
+      </c>
+      <c r="G12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>50</v>
+      </c>
+      <c r="J12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12">
+        <v>110.48</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q12">
+        <v>110048</v>
+      </c>
+      <c r="R12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13">
+        <v>6046</v>
+      </c>
+      <c r="D13">
+        <v>10648</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13">
+        <v>15</v>
+      </c>
+      <c r="I13">
+        <v>1300</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13">
+        <v>730.12</v>
+      </c>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13" t="s">
+        <v>74</v>
+      </c>
+      <c r="O13" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q13">
+        <v>111111</v>
+      </c>
+      <c r="R13" t="s">
+        <v>56</v>
+      </c>
+      <c r="S13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T13" t="s">
+        <v>26</v>
+      </c>
+      <c r="U13" t="s">
+        <v>26</v>
+      </c>
+      <c r="V13" t="s">
+        <v>26</v>
+      </c>
+      <c r="W13" t="s">
+        <v>26</v>
+      </c>
+      <c r="X13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14">
+        <v>6049</v>
+      </c>
+      <c r="D14">
+        <v>10628</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>200</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14">
+        <v>162</v>
+      </c>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14" t="s">
+        <v>40</v>
+      </c>
+      <c r="O14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q14">
+        <v>111111</v>
+      </c>
+      <c r="R14" t="s">
+        <v>26</v>
+      </c>
+      <c r="S14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15">
+        <v>6050</v>
+      </c>
+      <c r="D15">
+        <v>5951</v>
+      </c>
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>100</v>
+      </c>
+      <c r="J15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15">
+        <v>100</v>
+      </c>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15" t="s">
+        <v>74</v>
+      </c>
+      <c r="O15" t="s">
+        <v>74</v>
+      </c>
+      <c r="P15" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q15">
         <v>110018</v>
       </c>
-      <c r="R7" t="s">
-        <v>28</v>
+      <c r="R15" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>